<commit_message>
Bug fix: overlap penalty
(todo: verify)
</commit_message>
<xml_diff>
--- a/Examples/OverlapExample/OverlapExampleCosts.xlsx
+++ b/Examples/OverlapExample/OverlapExampleCosts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="55">
   <si>
     <t>Link cost for walk_access</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>overlap_variable</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>stochastic_dispersion</t>
   </si>
 </sst>
 </file>
@@ -214,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,8 +239,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -236,17 +254,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,17 +592,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="2" width="9.140625" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
+    <col min="3" max="10" width="9.140625" style="5"/>
+    <col min="11" max="11" width="9.140625" style="7"/>
+    <col min="12" max="13" width="9.140625" style="5"/>
+    <col min="14" max="14" width="13.5703125" style="5" customWidth="1"/>
+    <col min="15" max="19" width="9.140625" style="5"/>
+    <col min="20" max="21" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
@@ -571,7 +643,7 @@
       <c r="J1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>40</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -604,7 +676,7 @@
       <c r="U1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="10" t="s">
         <v>29</v>
       </c>
       <c r="W1" s="5" t="s">
@@ -648,7 +720,7 @@
       <c r="J2" s="5">
         <v>1</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="7">
         <v>0.33333333329999998</v>
       </c>
       <c r="L2" s="5">
@@ -667,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="5">
-        <v>31.566804019599999</v>
+        <v>30.252941176499998</v>
       </c>
       <c r="S2" s="5">
         <v>0</v>
@@ -678,8 +750,8 @@
       <c r="U2" s="5">
         <v>0</v>
       </c>
-      <c r="V2" s="5">
-        <v>0.118468877</v>
+      <c r="V2" s="11">
+        <v>0.33333333329999998</v>
       </c>
       <c r="W2" s="5">
         <v>1</v>
@@ -722,7 +794,7 @@
       <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="7">
         <v>0.33333333329999998</v>
       </c>
       <c r="L3" s="5">
@@ -735,7 +807,7 @@
         <v>24</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="5">
         <v>0</v>
@@ -752,8 +824,8 @@
       <c r="U3" s="5">
         <v>0</v>
       </c>
-      <c r="V3" s="5">
-        <v>0.44076556150000001</v>
+      <c r="V3" s="11">
+        <v>0.33333333329999998</v>
       </c>
       <c r="W3" s="5">
         <v>1</v>
@@ -796,7 +868,7 @@
       <c r="J4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="7">
         <v>0.33333333329999998</v>
       </c>
       <c r="L4" s="5">
@@ -809,35 +881,724 @@
         <v>19</v>
       </c>
       <c r="O4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0</v>
+      </c>
+      <c r="V4" s="11">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="W4" s="5">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L5" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S5" s="6">
+        <v>-0.83899905760000004</v>
+      </c>
+      <c r="T5" s="6">
+        <v>0</v>
+      </c>
+      <c r="U5" s="6">
+        <v>0</v>
+      </c>
+      <c r="V5" s="12">
+        <v>0.20133111479999999</v>
+      </c>
+      <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L6" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S6" s="6">
+        <v>-0.33647223659999997</v>
+      </c>
+      <c r="T6" s="6">
+        <v>0</v>
+      </c>
+      <c r="U6" s="6">
+        <v>0</v>
+      </c>
+      <c r="V6" s="12">
+        <v>0.3327787022</v>
+      </c>
+      <c r="W6" s="6">
+        <v>1</v>
+      </c>
+      <c r="X6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2</v>
+      </c>
+      <c r="I7" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L7" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="5">
-        <v>0</v>
-      </c>
-      <c r="R4" s="5">
-        <v>30.252941176499998</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
-        <v>0</v>
-      </c>
-      <c r="V4" s="5">
-        <v>0.44076556150000001</v>
-      </c>
-      <c r="W4" s="5">
-        <v>1</v>
-      </c>
-      <c r="X4" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>2</v>
-      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6">
+        <v>0</v>
+      </c>
+      <c r="R7" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S7" s="6">
+        <v>0</v>
+      </c>
+      <c r="T7" s="6">
+        <v>0</v>
+      </c>
+      <c r="U7" s="6">
+        <v>0</v>
+      </c>
+      <c r="V7" s="12">
+        <v>0.46589018300000001</v>
+      </c>
+      <c r="W7" s="6">
+        <v>1</v>
+      </c>
+      <c r="X7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L8" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0</v>
+      </c>
+      <c r="R8" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S8" s="5">
+        <v>-0.48745846409999999</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0</v>
+      </c>
+      <c r="V8" s="11">
+        <v>0.27562082300000001</v>
+      </c>
+      <c r="W8" s="5">
+        <v>1</v>
+      </c>
+      <c r="X8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L9" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S9" s="5">
+        <v>-0.48745846409999999</v>
+      </c>
+      <c r="T9" s="5">
+        <v>0</v>
+      </c>
+      <c r="U9" s="5">
+        <v>0</v>
+      </c>
+      <c r="V9" s="11">
+        <v>0.27562082300000001</v>
+      </c>
+      <c r="W9" s="5">
+        <v>1</v>
+      </c>
+      <c r="X9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L10" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="11">
+        <v>0.44875835390000002</v>
+      </c>
+      <c r="W10" s="5">
+        <v>1</v>
+      </c>
+      <c r="X10" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L11" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6">
+        <v>0</v>
+      </c>
+      <c r="R11" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S11" s="6">
+        <v>-0.31223204189999998</v>
+      </c>
+      <c r="T11" s="6">
+        <v>0</v>
+      </c>
+      <c r="U11" s="6">
+        <v>0</v>
+      </c>
+      <c r="V11" s="12">
+        <v>0.29704690210000001</v>
+      </c>
+      <c r="W11" s="6">
+        <v>1</v>
+      </c>
+      <c r="X11" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L12" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6">
+        <v>0</v>
+      </c>
+      <c r="R12" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S12" s="6">
+        <v>-0.31223204189999998</v>
+      </c>
+      <c r="T12" s="6">
+        <v>0</v>
+      </c>
+      <c r="U12" s="6">
+        <v>0</v>
+      </c>
+      <c r="V12" s="12">
+        <v>0.29704690210000001</v>
+      </c>
+      <c r="W12" s="6">
+        <v>1</v>
+      </c>
+      <c r="X12" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
+      <c r="I13" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.33333333329999998</v>
+      </c>
+      <c r="L13" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6">
+        <v>0</v>
+      </c>
+      <c r="R13" s="6">
+        <v>30.252941176499998</v>
+      </c>
+      <c r="S13" s="6">
+        <v>0</v>
+      </c>
+      <c r="T13" s="6">
+        <v>0</v>
+      </c>
+      <c r="U13" s="6">
+        <v>0</v>
+      </c>
+      <c r="V13" s="13">
+        <v>0.40590619570000003</v>
+      </c>
+      <c r="W13" s="6">
+        <v>1</v>
+      </c>
+      <c r="X13" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V20" s="7"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V21" s="7"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="V22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>